<commit_message>
Updated existing code for Heifers
</commit_message>
<xml_diff>
--- a/src/nasem_dairy/data/Variable List.xlsx
+++ b/src/nasem_dairy/data/Variable List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoguelphca-my.sharepoint.com/personal/innesd_uoguelph_ca/Documents/UoG/UoG Python/NASEM-Model-Python/src/nasem_dairy/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoguelphca-my.sharepoint.com/personal/bfieguth_uoguelph_ca/Documents/NASEM-Model-Python/src/nasem_dairy/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{9502600B-C053-428D-8A19-8D6EB97F7AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{554B041A-33FE-8E49-84E8-57CB6B497A0C}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{9502600B-C053-428D-8A19-8D6EB97F7AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3492CED-783E-4D6E-BEA5-10FB931CF24C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="760" windowWidth="29040" windowHeight="15840" xr2:uid="{53988E5A-922A-4D43-857E-3D1DAEEFC7AC}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{53988E5A-922A-4D43-857E-3D1DAEEFC7AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="535">
   <si>
     <t>Variable Name</t>
   </si>
@@ -1618,6 +1618,30 @@
   </si>
   <si>
     <t>Predicted milk protein content, %</t>
+  </si>
+  <si>
+    <t>Diff_MPuse_g</t>
+  </si>
+  <si>
+    <t>An_MEIn_approx</t>
+  </si>
+  <si>
+    <t>Frm_MPUse_g_Trg</t>
+  </si>
+  <si>
+    <t>Kg_MP_NP_Trg</t>
+  </si>
+  <si>
+    <t>Min_MPuse_g</t>
+  </si>
+  <si>
+    <t>Frm_NPgain_g</t>
+  </si>
+  <si>
+    <t>Rsrv_NPgain_g</t>
+  </si>
+  <si>
+    <t>Rsrv_MPUse_g_Trg</t>
   </si>
 </sst>
 </file>
@@ -1692,7 +1716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1704,7 +1728,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2120,23 +2143,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CBC222-87FC-4995-A1F1-81937BD3329A}">
-  <dimension ref="A1:G234"/>
+  <dimension ref="A1:G243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A218" zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F233" sqref="F233:F234"/>
+    <sheetView tabSelected="1" topLeftCell="A224" zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D237" sqref="D237:D243"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="20.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5" customWidth="1"/>
+    <col min="4" max="4" width="14.46484375" customWidth="1"/>
+    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.1328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>292</v>
       </c>
@@ -2159,7 +2182,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2179,7 +2202,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2199,7 +2222,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2219,7 +2242,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2239,7 +2262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2259,7 +2282,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2279,7 +2302,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2299,7 +2322,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2319,7 +2342,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2339,7 +2362,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2359,7 +2382,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2379,7 +2402,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2399,7 +2422,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2419,7 +2442,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2439,7 +2462,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2459,7 +2482,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2479,7 +2502,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2499,7 +2522,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2519,7 +2542,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2539,7 +2562,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2559,7 +2582,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2579,7 +2602,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2599,7 +2622,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2619,7 +2642,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2639,7 +2662,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2659,7 +2682,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2683,7 +2706,7 @@
         <v>Fd_NDF_kg/d</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2703,7 +2726,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2723,7 +2746,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2743,7 +2766,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2763,7 +2786,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2783,7 +2806,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2803,7 +2826,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2823,7 +2846,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2843,7 +2866,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2863,7 +2886,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2883,7 +2906,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2903,7 +2926,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2923,7 +2946,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2943,7 +2966,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2963,7 +2986,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2983,7 +3006,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3003,7 +3026,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3023,7 +3046,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3043,7 +3066,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3063,7 +3086,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3083,7 +3106,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3103,7 +3126,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3123,7 +3146,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3143,7 +3166,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3163,7 +3186,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3183,7 +3206,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3203,7 +3226,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3223,7 +3246,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3243,7 +3266,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3263,7 +3286,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3283,7 +3306,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3303,7 +3326,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3323,7 +3346,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3347,7 +3370,7 @@
         <v>Fd_ForNDF</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3367,7 +3390,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3387,7 +3410,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3407,7 +3430,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3431,7 +3454,7 @@
         <v>Dt_RDPIn</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3451,7 +3474,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3471,7 +3494,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3491,7 +3514,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3511,7 +3534,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3531,7 +3554,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3551,7 +3574,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3571,7 +3594,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3591,7 +3614,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3611,7 +3634,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3631,7 +3654,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3651,7 +3674,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3668,7 +3691,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3685,7 +3708,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3702,7 +3725,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3719,7 +3742,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3736,7 +3759,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3756,7 +3779,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3776,7 +3799,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3796,7 +3819,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3813,7 +3836,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3833,7 +3856,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3850,7 +3873,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3867,7 +3890,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3884,7 +3907,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3904,7 +3927,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3921,7 +3944,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3941,7 +3964,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3961,7 +3984,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>92</v>
       </c>
@@ -3978,7 +4001,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94">
         <v>93</v>
       </c>
@@ -3998,7 +4021,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4015,7 +4038,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4035,7 +4058,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4052,7 +4075,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4072,7 +4095,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4089,7 +4112,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4109,7 +4132,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4129,7 +4152,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4149,7 +4172,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4169,7 +4192,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4189,7 +4212,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4209,7 +4232,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4229,7 +4252,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4249,7 +4272,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4269,7 +4292,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4289,7 +4312,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110">
         <v>109</v>
       </c>
@@ -4309,7 +4332,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4329,7 +4352,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A112">
         <v>111</v>
       </c>
@@ -4346,7 +4369,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4363,7 +4386,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4383,7 +4406,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4403,7 +4426,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4423,7 +4446,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4443,7 +4466,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A118">
         <v>117</v>
       </c>
@@ -4463,7 +4486,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A119">
         <v>118</v>
       </c>
@@ -4480,7 +4503,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A120">
         <v>119</v>
       </c>
@@ -4500,7 +4523,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A121">
         <v>120</v>
       </c>
@@ -4520,7 +4543,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A122">
         <v>121</v>
       </c>
@@ -4540,7 +4563,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A123">
         <v>122</v>
       </c>
@@ -4557,7 +4580,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4577,7 +4600,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A125">
         <v>124</v>
       </c>
@@ -4594,7 +4617,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A126">
         <v>125</v>
       </c>
@@ -4614,7 +4637,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A127">
         <v>126</v>
       </c>
@@ -4634,7 +4657,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A128">
         <v>127</v>
       </c>
@@ -4651,7 +4674,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A129">
         <v>128</v>
       </c>
@@ -4671,7 +4694,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A130">
         <v>129</v>
       </c>
@@ -4691,7 +4714,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A131">
         <v>130</v>
       </c>
@@ -4711,7 +4734,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A132">
         <v>131</v>
       </c>
@@ -4728,7 +4751,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A133">
         <v>132</v>
       </c>
@@ -4748,7 +4771,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A134">
         <v>133</v>
       </c>
@@ -4765,7 +4788,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A135">
         <v>134</v>
       </c>
@@ -4785,7 +4808,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A136">
         <v>135</v>
       </c>
@@ -4805,7 +4828,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A137">
         <v>136</v>
       </c>
@@ -4822,7 +4845,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A138">
         <v>137</v>
       </c>
@@ -4842,7 +4865,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A139">
         <v>138</v>
       </c>
@@ -4862,7 +4885,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A140">
         <v>139</v>
       </c>
@@ -4879,7 +4902,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A141">
         <v>140</v>
       </c>
@@ -4896,7 +4919,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A142">
         <v>141</v>
       </c>
@@ -4913,7 +4936,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A143">
         <v>142</v>
       </c>
@@ -4933,7 +4956,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A144">
         <v>143</v>
       </c>
@@ -4953,7 +4976,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A145">
         <v>144</v>
       </c>
@@ -4973,7 +4996,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A146">
         <v>145</v>
       </c>
@@ -4993,7 +5016,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A147">
         <v>146</v>
       </c>
@@ -5013,7 +5036,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A148">
         <v>147</v>
       </c>
@@ -5030,7 +5053,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A149">
         <v>148</v>
       </c>
@@ -5050,7 +5073,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A150">
         <v>149</v>
       </c>
@@ -5070,7 +5093,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A151">
         <v>150</v>
       </c>
@@ -5087,7 +5110,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A152">
         <v>151</v>
       </c>
@@ -5104,7 +5127,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A153">
         <v>152</v>
       </c>
@@ -5124,7 +5147,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A154">
         <v>153</v>
       </c>
@@ -5144,7 +5167,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A155">
         <v>154</v>
       </c>
@@ -5164,7 +5187,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A156">
         <v>155</v>
       </c>
@@ -5184,7 +5207,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A157">
         <v>156</v>
       </c>
@@ -5201,7 +5224,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A158">
         <v>157</v>
       </c>
@@ -5221,7 +5244,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A159">
         <v>158</v>
       </c>
@@ -5241,7 +5264,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A160">
         <v>159</v>
       </c>
@@ -5261,7 +5284,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A161">
         <v>160</v>
       </c>
@@ -5281,7 +5304,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A162">
         <v>161</v>
       </c>
@@ -5301,7 +5324,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A163">
         <v>162</v>
       </c>
@@ -5321,7 +5344,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A164">
         <v>163</v>
       </c>
@@ -5341,7 +5364,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A165">
         <v>164</v>
       </c>
@@ -5361,7 +5384,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A166">
         <v>165</v>
       </c>
@@ -5381,7 +5404,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A167">
         <v>166</v>
       </c>
@@ -5401,7 +5424,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A168">
         <v>167</v>
       </c>
@@ -5421,7 +5444,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A169">
         <v>168</v>
       </c>
@@ -5445,7 +5468,7 @@
         <v>Rsrv_Gain_empty</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A170">
         <v>169</v>
       </c>
@@ -5465,7 +5488,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A171">
         <v>170</v>
       </c>
@@ -5485,7 +5508,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A172">
         <v>171</v>
       </c>
@@ -5505,7 +5528,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A173">
         <v>172</v>
       </c>
@@ -5525,7 +5548,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A174">
         <v>173</v>
       </c>
@@ -5545,7 +5568,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A175">
         <v>174</v>
       </c>
@@ -5565,7 +5588,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A176">
         <v>175</v>
       </c>
@@ -5585,7 +5608,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A177">
         <v>176</v>
       </c>
@@ -5609,7 +5632,7 @@
         <v>Frm_Gain</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A178">
         <v>177</v>
       </c>
@@ -5633,7 +5656,7 @@
         <v>Frm_Gain_empty</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A179">
         <v>178</v>
       </c>
@@ -5653,7 +5676,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A180">
         <v>179</v>
       </c>
@@ -5677,7 +5700,7 @@
         <v>NPGain_FrmGain</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A181">
         <v>180</v>
       </c>
@@ -5697,7 +5720,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A182">
         <v>181</v>
       </c>
@@ -5717,7 +5740,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A183">
         <v>182</v>
       </c>
@@ -5737,7 +5760,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A184">
         <v>183</v>
       </c>
@@ -5757,7 +5780,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A185">
         <v>184</v>
       </c>
@@ -5777,7 +5800,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A186">
         <v>185</v>
       </c>
@@ -5797,7 +5820,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A187">
         <v>186</v>
       </c>
@@ -5817,7 +5840,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A188">
         <v>187</v>
       </c>
@@ -5837,7 +5860,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A189">
         <v>188</v>
       </c>
@@ -5860,7 +5883,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A190">
         <v>189</v>
       </c>
@@ -5880,7 +5903,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A191">
         <v>190</v>
       </c>
@@ -5900,7 +5923,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A192">
         <v>191</v>
       </c>
@@ -5920,7 +5943,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A193">
         <v>192</v>
       </c>
@@ -5944,7 +5967,7 @@
         <v>An_NDF</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A194">
         <v>193</v>
       </c>
@@ -5968,7 +5991,7 @@
         <v>Fe_CPend_g</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A195">
         <v>194</v>
       </c>
@@ -5992,7 +6015,7 @@
         <v>Fe_CPend</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A196">
         <v>195</v>
       </c>
@@ -6012,7 +6035,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A197">
         <v>196</v>
       </c>
@@ -6032,7 +6055,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A198">
         <v>197</v>
       </c>
@@ -6052,7 +6075,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A199">
         <v>198</v>
       </c>
@@ -6076,7 +6099,7 @@
         <v>Scrf_CP_g</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A200">
         <v>199</v>
       </c>
@@ -6096,7 +6119,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A201">
         <v>200</v>
       </c>
@@ -6116,7 +6139,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A202">
         <v>201</v>
       </c>
@@ -6136,7 +6159,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A203">
         <v>202</v>
       </c>
@@ -6156,7 +6179,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A204">
         <v>203</v>
       </c>
@@ -6176,7 +6199,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A205">
         <v>204</v>
       </c>
@@ -6196,7 +6219,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A206">
         <v>205</v>
       </c>
@@ -6220,7 +6243,7 @@
         <v>CPGain_FrmGain</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A207">
         <v>206</v>
       </c>
@@ -6244,7 +6267,7 @@
         <v>NPGain_FrmGain</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A208">
         <v>207</v>
       </c>
@@ -6268,7 +6291,7 @@
         <v>Frm_Gain</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A209">
         <v>208</v>
       </c>
@@ -6292,7 +6315,7 @@
         <v>Frm_Gain_empty</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A210">
         <v>209</v>
       </c>
@@ -6316,7 +6339,7 @@
         <v>Frm_NPgain</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A211">
         <v>210</v>
       </c>
@@ -6340,7 +6363,7 @@
         <v>NPGain_RsrvGain</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A212">
         <v>211</v>
       </c>
@@ -6364,7 +6387,7 @@
         <v>Rsrv_Gain_empty</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A213">
         <v>212</v>
       </c>
@@ -6388,7 +6411,7 @@
         <v>Rsrv_NPgain</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A214">
         <v>213</v>
       </c>
@@ -6412,7 +6435,7 @@
         <v>Body_NPgain</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A215">
         <v>214</v>
       </c>
@@ -6432,7 +6455,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A216">
         <v>215</v>
       </c>
@@ -6452,7 +6475,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A217">
         <v>216</v>
       </c>
@@ -6476,7 +6499,7 @@
         <v>Gest_NCPgain_g</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A218">
         <v>217</v>
       </c>
@@ -6500,7 +6523,7 @@
         <v>Gest_NPgain_g</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A219">
         <v>218</v>
       </c>
@@ -6524,7 +6547,7 @@
         <v>Gest_NPuse_g</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A220">
         <v>219</v>
       </c>
@@ -6544,7 +6567,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A221">
         <v>220</v>
       </c>
@@ -6564,7 +6587,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A222">
         <v>221</v>
       </c>
@@ -6584,7 +6607,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A223">
         <v>222</v>
       </c>
@@ -6601,7 +6624,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A224">
         <v>223</v>
       </c>
@@ -6621,7 +6644,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A225">
         <v>224</v>
       </c>
@@ -6641,7 +6664,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A226">
         <v>225</v>
       </c>
@@ -6661,7 +6684,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A227">
         <v>226</v>
       </c>
@@ -6681,7 +6704,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A228">
         <v>227</v>
       </c>
@@ -6701,7 +6724,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A229">
         <v>228</v>
       </c>
@@ -6721,7 +6744,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A230">
         <v>229</v>
       </c>
@@ -6741,7 +6764,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A231">
         <v>230</v>
       </c>
@@ -6761,7 +6784,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A232">
         <v>231</v>
       </c>
@@ -6781,28 +6804,158 @@
         <v>520</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B233" t="s">
         <v>523</v>
       </c>
-      <c r="C233" s="7"/>
       <c r="F233" t="s">
         <v>524</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B234" t="s">
         <v>525</v>
       </c>
-      <c r="C234" s="7"/>
       <c r="F234" t="s">
         <v>526</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A235">
+        <v>232</v>
+      </c>
+      <c r="B235" s="4" t="s">
+        <v>527</v>
+      </c>
+      <c r="C235" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="D235" t="s">
+        <v>97</v>
+      </c>
+      <c r="E235">
+        <v>2689</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A236">
+        <v>233</v>
+      </c>
+      <c r="B236" s="4" t="s">
+        <v>528</v>
+      </c>
+      <c r="C236" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="D236" t="s">
+        <v>97</v>
+      </c>
+      <c r="E236">
+        <v>2686</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A237">
+        <v>234</v>
+      </c>
+      <c r="B237" s="4" t="s">
+        <v>529</v>
+      </c>
+      <c r="C237" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="D237" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A238">
+        <v>235</v>
+      </c>
+      <c r="B238" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="C238" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="D238" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A239">
+        <v>236</v>
+      </c>
+      <c r="B239" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="C239" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="D239" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A240">
+        <v>237</v>
+      </c>
+      <c r="B240" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="C240" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="D240" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A241">
+        <v>238</v>
+      </c>
+      <c r="B241" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="C241" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="D241" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A242">
+        <v>239</v>
+      </c>
+      <c r="B242" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="C242" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="D242" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A243">
+        <v>240</v>
+      </c>
+      <c r="B243" s="4" t="s">
+        <v>534</v>
+      </c>
+      <c r="C243" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="D243" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
@@ -6817,14 +6970,14 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="67.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>293</v>
       </c>
@@ -6835,7 +6988,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>294</v>
       </c>
@@ -6846,7 +6999,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>296</v>
       </c>
@@ -6857,7 +7010,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>298</v>
       </c>
@@ -6868,7 +7021,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>299</v>
       </c>
@@ -6879,7 +7032,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>301</v>
       </c>
@@ -6890,7 +7043,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>302</v>
       </c>
@@ -6901,7 +7054,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>309</v>
       </c>
@@ -6912,7 +7065,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>311</v>
       </c>
@@ -6923,7 +7076,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>314</v>
       </c>
@@ -6934,7 +7087,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>318</v>
       </c>
@@ -6945,7 +7098,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>320</v>
       </c>
@@ -6956,7 +7109,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>322</v>
       </c>
@@ -6967,7 +7120,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>323</v>
       </c>
@@ -6978,7 +7131,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>325</v>
       </c>
@@ -6989,7 +7142,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>329</v>
       </c>
@@ -7000,7 +7153,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>331</v>
       </c>
@@ -7011,7 +7164,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>333</v>
       </c>
@@ -7022,7 +7175,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>335</v>
       </c>
@@ -7033,7 +7186,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>337</v>
       </c>
@@ -7044,7 +7197,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>339</v>
       </c>

</xml_diff>

<commit_message>
Added heifer growth calculations
</commit_message>
<xml_diff>
--- a/src/nasem_dairy/data/Variable List.xlsx
+++ b/src/nasem_dairy/data/Variable List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoguelphca-my.sharepoint.com/personal/bfieguth_uoguelph_ca/Documents/NASEM-Model-Python/src/nasem_dairy/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Braeden\OneDrive - University of Guelph\NASEM-Model-Python\src\nasem_dairy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{9502600B-C053-428D-8A19-8D6EB97F7AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3492CED-783E-4D6E-BEA5-10FB931CF24C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7F192A-A044-42C7-8DE1-AA521F9111D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{53988E5A-922A-4D43-857E-3D1DAEEFC7AC}"/>
+    <workbookView xWindow="-28920" yWindow="810" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{53988E5A-922A-4D43-857E-3D1DAEEFC7AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="538">
   <si>
     <t>Variable Name</t>
   </si>
@@ -1642,6 +1642,15 @@
   </si>
   <si>
     <t>Rsrv_MPUse_g_Trg</t>
+  </si>
+  <si>
+    <t>An_PhysState</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>Lactating Cow, Heifer, Dry Cow or Calf</t>
   </si>
 </sst>
 </file>
@@ -1835,8 +1844,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{80C4780E-C903-42C8-A8A5-844980E5F27B}" name="Table2" displayName="Table2" ref="A1:C21" totalsRowShown="0">
-  <autoFilter ref="A1:C21" xr:uid="{80C4780E-C903-42C8-A8A5-844980E5F27B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{80C4780E-C903-42C8-A8A5-844980E5F27B}" name="Table2" displayName="Table2" ref="A1:C22" totalsRowShown="0">
+  <autoFilter ref="A1:C22" xr:uid="{80C4780E-C903-42C8-A8A5-844980E5F27B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{B4C59711-313F-4930-B87F-432F2876F0BC}" name="Name"/>
     <tableColumn id="2" xr3:uid="{A4544BC0-902D-47F2-AB54-0B1C12C8AD1C}" name="Units"/>
@@ -2145,21 +2154,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CBC222-87FC-4995-A1F1-81937BD3329A}">
   <dimension ref="A1:G243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A224" zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D237" sqref="D237:D243"/>
+    <sheetView topLeftCell="A238" zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F241" sqref="F241"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.46484375" customWidth="1"/>
-    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.46484375" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>292</v>
       </c>
@@ -2182,7 +2191,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2202,7 +2211,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2222,7 +2231,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2242,7 +2251,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2262,7 +2271,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2282,7 +2291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2302,7 +2311,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2322,7 +2331,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2342,7 +2351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2362,7 +2371,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2382,7 +2391,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2402,7 +2411,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2422,7 +2431,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2442,7 +2451,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2462,7 +2471,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2482,7 +2491,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2502,7 +2511,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2522,7 +2531,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2542,7 +2551,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2562,7 +2571,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2582,7 +2591,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2602,7 +2611,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2622,7 +2631,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2642,7 +2651,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2662,7 +2671,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2682,7 +2691,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2706,7 +2715,7 @@
         <v>Fd_NDF_kg/d</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2726,7 +2735,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2746,7 +2755,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2766,7 +2775,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2786,7 +2795,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2806,7 +2815,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2826,7 +2835,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2846,7 +2855,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2866,7 +2875,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2886,7 +2895,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2906,7 +2915,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2926,7 +2935,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2946,7 +2955,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2966,7 +2975,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2986,7 +2995,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3006,7 +3015,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3026,7 +3035,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3046,7 +3055,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3066,7 +3075,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3086,7 +3095,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3106,7 +3115,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3126,7 +3135,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3146,7 +3155,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3166,7 +3175,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3186,7 +3195,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3206,7 +3215,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3226,7 +3235,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3246,7 +3255,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3266,7 +3275,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3286,7 +3295,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3306,7 +3315,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3326,7 +3335,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3346,7 +3355,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3370,7 +3379,7 @@
         <v>Fd_ForNDF</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3390,7 +3399,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3410,7 +3419,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3430,7 +3439,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3454,7 +3463,7 @@
         <v>Dt_RDPIn</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3474,7 +3483,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3494,7 +3503,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3514,7 +3523,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3534,7 +3543,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3554,7 +3563,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3574,7 +3583,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3594,7 +3603,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3614,7 +3623,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3634,7 +3643,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3654,7 +3663,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3674,7 +3683,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3691,7 +3700,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3708,7 +3717,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3725,7 +3734,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3742,7 +3751,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3759,7 +3768,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3779,7 +3788,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3799,7 +3808,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3819,7 +3828,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3836,7 +3845,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3856,7 +3865,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3873,7 +3882,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3890,7 +3899,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3907,7 +3916,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3927,7 +3936,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3944,7 +3953,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3964,7 +3973,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3984,7 +3993,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4001,7 +4010,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4021,7 +4030,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4038,7 +4047,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4058,7 +4067,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4075,7 +4084,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4095,7 +4104,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4112,7 +4121,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4132,7 +4141,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4152,7 +4161,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4172,7 +4181,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4192,7 +4201,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4212,7 +4221,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4232,7 +4241,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4252,7 +4261,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4272,7 +4281,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4292,7 +4301,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4312,7 +4321,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -4332,7 +4341,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4352,7 +4361,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -4369,7 +4378,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4386,7 +4395,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4406,7 +4415,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4426,7 +4435,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4446,7 +4455,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4466,7 +4475,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -4486,7 +4495,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -4503,7 +4512,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -4523,7 +4532,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -4543,7 +4552,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -4563,7 +4572,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -4580,7 +4589,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4600,7 +4609,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -4617,7 +4626,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -4637,7 +4646,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -4657,7 +4666,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -4674,7 +4683,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -4694,7 +4703,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -4714,7 +4723,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -4734,7 +4743,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -4751,7 +4760,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -4771,7 +4780,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -4788,7 +4797,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -4808,7 +4817,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -4828,7 +4837,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -4845,7 +4854,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -4865,7 +4874,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -4885,7 +4894,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -4902,7 +4911,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -4919,7 +4928,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -4936,7 +4945,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -4956,7 +4965,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -4976,7 +4985,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -4996,7 +5005,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -5016,7 +5025,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -5036,7 +5045,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -5053,7 +5062,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -5073,7 +5082,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -5093,7 +5102,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -5110,7 +5119,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -5127,7 +5136,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -5147,7 +5156,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -5167,7 +5176,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -5187,7 +5196,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -5207,7 +5216,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -5224,7 +5233,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -5244,7 +5253,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -5264,7 +5273,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -5284,7 +5293,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -5304,7 +5313,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -5324,7 +5333,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
@@ -5344,7 +5353,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
@@ -5364,7 +5373,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
@@ -5384,7 +5393,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
@@ -5404,7 +5413,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
@@ -5424,7 +5433,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
@@ -5444,7 +5453,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -5468,7 +5477,7 @@
         <v>Rsrv_Gain_empty</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
@@ -5488,7 +5497,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
@@ -5508,7 +5517,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
@@ -5528,7 +5537,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
@@ -5548,7 +5557,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
@@ -5568,7 +5577,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
@@ -5588,7 +5597,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
@@ -5608,7 +5617,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -5632,7 +5641,7 @@
         <v>Frm_Gain</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
@@ -5656,7 +5665,7 @@
         <v>Frm_Gain_empty</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -5676,7 +5685,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
@@ -5700,7 +5709,7 @@
         <v>NPGain_FrmGain</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
@@ -5720,7 +5729,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
@@ -5740,7 +5749,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
@@ -5760,7 +5769,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
@@ -5780,7 +5789,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
@@ -5800,7 +5809,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
@@ -5820,7 +5829,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
@@ -5840,7 +5849,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
@@ -5860,7 +5869,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
@@ -5883,7 +5892,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
@@ -5903,7 +5912,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
@@ -5923,7 +5932,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
@@ -5943,7 +5952,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
@@ -5967,7 +5976,7 @@
         <v>An_NDF</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
@@ -5991,7 +6000,7 @@
         <v>Fe_CPend_g</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
@@ -6015,7 +6024,7 @@
         <v>Fe_CPend</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
@@ -6035,7 +6044,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
@@ -6055,7 +6064,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
@@ -6075,7 +6084,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
@@ -6099,7 +6108,7 @@
         <v>Scrf_CP_g</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
@@ -6119,7 +6128,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
@@ -6139,7 +6148,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>201</v>
       </c>
@@ -6159,7 +6168,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>202</v>
       </c>
@@ -6179,7 +6188,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>203</v>
       </c>
@@ -6199,7 +6208,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>204</v>
       </c>
@@ -6219,7 +6228,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>205</v>
       </c>
@@ -6243,7 +6252,7 @@
         <v>CPGain_FrmGain</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>206</v>
       </c>
@@ -6267,7 +6276,7 @@
         <v>NPGain_FrmGain</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>207</v>
       </c>
@@ -6291,7 +6300,7 @@
         <v>Frm_Gain</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>208</v>
       </c>
@@ -6315,7 +6324,7 @@
         <v>Frm_Gain_empty</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>209</v>
       </c>
@@ -6339,7 +6348,7 @@
         <v>Frm_NPgain</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>210</v>
       </c>
@@ -6363,7 +6372,7 @@
         <v>NPGain_RsrvGain</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>211</v>
       </c>
@@ -6387,7 +6396,7 @@
         <v>Rsrv_Gain_empty</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>212</v>
       </c>
@@ -6411,7 +6420,7 @@
         <v>Rsrv_NPgain</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>213</v>
       </c>
@@ -6435,7 +6444,7 @@
         <v>Body_NPgain</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>214</v>
       </c>
@@ -6455,7 +6464,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>215</v>
       </c>
@@ -6475,7 +6484,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>216</v>
       </c>
@@ -6499,7 +6508,7 @@
         <v>Gest_NCPgain_g</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>217</v>
       </c>
@@ -6523,7 +6532,7 @@
         <v>Gest_NPgain_g</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>218</v>
       </c>
@@ -6547,7 +6556,7 @@
         <v>Gest_NPuse_g</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>219</v>
       </c>
@@ -6567,7 +6576,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>220</v>
       </c>
@@ -6587,7 +6596,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>221</v>
       </c>
@@ -6607,7 +6616,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>222</v>
       </c>
@@ -6624,7 +6633,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>223</v>
       </c>
@@ -6644,7 +6653,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>224</v>
       </c>
@@ -6664,7 +6673,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>225</v>
       </c>
@@ -6684,7 +6693,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>226</v>
       </c>
@@ -6704,7 +6713,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>227</v>
       </c>
@@ -6724,7 +6733,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>228</v>
       </c>
@@ -6744,7 +6753,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>229</v>
       </c>
@@ -6764,7 +6773,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>230</v>
       </c>
@@ -6784,7 +6793,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>231</v>
       </c>
@@ -6804,7 +6813,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
         <v>523</v>
       </c>
@@ -6812,7 +6821,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
         <v>525</v>
       </c>
@@ -6820,7 +6829,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>232</v>
       </c>
@@ -6837,7 +6846,7 @@
         <v>2689</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>233</v>
       </c>
@@ -6854,7 +6863,7 @@
         <v>2686</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>234</v>
       </c>
@@ -6868,7 +6877,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>235</v>
       </c>
@@ -6882,7 +6891,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>236</v>
       </c>
@@ -6896,7 +6905,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>237</v>
       </c>
@@ -6910,7 +6919,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>238</v>
       </c>
@@ -6924,7 +6933,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>239</v>
       </c>
@@ -6938,7 +6947,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>240</v>
       </c>
@@ -6964,20 +6973,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750FF422-2362-464E-8AF6-B12F418D3E4F}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="67.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="67.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>293</v>
       </c>
@@ -6988,7 +6997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>294</v>
       </c>
@@ -6999,7 +7008,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>296</v>
       </c>
@@ -7010,7 +7019,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>298</v>
       </c>
@@ -7021,7 +7030,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>299</v>
       </c>
@@ -7032,7 +7041,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>301</v>
       </c>
@@ -7043,7 +7052,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>302</v>
       </c>
@@ -7054,7 +7063,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>309</v>
       </c>
@@ -7065,7 +7074,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>311</v>
       </c>
@@ -7076,7 +7085,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>314</v>
       </c>
@@ -7087,7 +7096,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>318</v>
       </c>
@@ -7098,7 +7107,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>320</v>
       </c>
@@ -7109,7 +7118,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>322</v>
       </c>
@@ -7120,7 +7129,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>323</v>
       </c>
@@ -7131,7 +7140,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>325</v>
       </c>
@@ -7142,7 +7151,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>329</v>
       </c>
@@ -7153,7 +7162,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>331</v>
       </c>
@@ -7164,7 +7173,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>333</v>
       </c>
@@ -7175,7 +7184,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>335</v>
       </c>
@@ -7186,7 +7195,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>337</v>
       </c>
@@ -7197,7 +7206,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>339</v>
       </c>
@@ -7206,6 +7215,17 @@
       </c>
       <c r="C21" t="s">
         <v>340</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>535</v>
+      </c>
+      <c r="B22" t="s">
+        <v>536</v>
+      </c>
+      <c r="C22" t="s">
+        <v>537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mineral and vitamin requirements
</commit_message>
<xml_diff>
--- a/src/nasem_dairy/data/Variable List.xlsx
+++ b/src/nasem_dairy/data/Variable List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoguelphca-my.sharepoint.com/personal/bfieguth_uoguelph_ca/Documents/NASEM-Model-Python/src/nasem_dairy/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Braeden\OneDrive - University of Guelph\NASEM-Model-Python\src\nasem_dairy\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{9502600B-C053-428D-8A19-8D6EB97F7AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3492CED-783E-4D6E-BEA5-10FB931CF24C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7F192A-A044-42C7-8DE1-AA521F9111D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{53988E5A-922A-4D43-857E-3D1DAEEFC7AC}"/>
+    <workbookView xWindow="-28920" yWindow="810" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{53988E5A-922A-4D43-857E-3D1DAEEFC7AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1091" uniqueCount="538">
   <si>
     <t>Variable Name</t>
   </si>
@@ -1642,6 +1642,15 @@
   </si>
   <si>
     <t>Rsrv_MPUse_g_Trg</t>
+  </si>
+  <si>
+    <t>An_PhysState</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>Lactating Cow, Heifer, Dry Cow or Calf</t>
   </si>
 </sst>
 </file>
@@ -1835,8 +1844,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{80C4780E-C903-42C8-A8A5-844980E5F27B}" name="Table2" displayName="Table2" ref="A1:C21" totalsRowShown="0">
-  <autoFilter ref="A1:C21" xr:uid="{80C4780E-C903-42C8-A8A5-844980E5F27B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{80C4780E-C903-42C8-A8A5-844980E5F27B}" name="Table2" displayName="Table2" ref="A1:C22" totalsRowShown="0">
+  <autoFilter ref="A1:C22" xr:uid="{80C4780E-C903-42C8-A8A5-844980E5F27B}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{B4C59711-313F-4930-B87F-432F2876F0BC}" name="Name"/>
     <tableColumn id="2" xr3:uid="{A4544BC0-902D-47F2-AB54-0B1C12C8AD1C}" name="Units"/>
@@ -2145,21 +2154,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3CBC222-87FC-4995-A1F1-81937BD3329A}">
   <dimension ref="A1:G243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A224" zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D237" sqref="D237:D243"/>
+    <sheetView topLeftCell="A238" zoomScale="150" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F241" sqref="F241"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.46484375" customWidth="1"/>
-    <col min="5" max="5" width="15.1328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.46484375" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>292</v>
       </c>
@@ -2182,7 +2191,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2202,7 +2211,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2222,7 +2231,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2242,7 +2251,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2262,7 +2271,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2282,7 +2291,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2302,7 +2311,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2322,7 +2331,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2342,7 +2351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2362,7 +2371,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2382,7 +2391,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2402,7 +2411,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2422,7 +2431,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2442,7 +2451,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2462,7 +2471,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2482,7 +2491,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2502,7 +2511,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2522,7 +2531,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2542,7 +2551,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2562,7 +2571,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2582,7 +2591,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2602,7 +2611,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2622,7 +2631,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2642,7 +2651,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2662,7 +2671,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2682,7 +2691,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2706,7 +2715,7 @@
         <v>Fd_NDF_kg/d</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2726,7 +2735,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2746,7 +2755,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2766,7 +2775,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2786,7 +2795,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2806,7 +2815,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2826,7 +2835,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2846,7 +2855,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2866,7 +2875,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2886,7 +2895,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2906,7 +2915,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2926,7 +2935,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2946,7 +2955,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2966,7 +2975,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2986,7 +2995,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3006,7 +3015,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3026,7 +3035,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3046,7 +3055,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3066,7 +3075,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3086,7 +3095,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3106,7 +3115,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3126,7 +3135,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3146,7 +3155,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3166,7 +3175,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3186,7 +3195,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3206,7 +3215,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3226,7 +3235,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3246,7 +3255,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3266,7 +3275,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3286,7 +3295,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3306,7 +3315,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3326,7 +3335,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3346,7 +3355,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -3370,7 +3379,7 @@
         <v>Fd_ForNDF</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3390,7 +3399,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3410,7 +3419,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3430,7 +3439,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3454,7 +3463,7 @@
         <v>Dt_RDPIn</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3474,7 +3483,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -3494,7 +3503,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -3514,7 +3523,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -3534,7 +3543,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -3554,7 +3563,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -3574,7 +3583,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -3594,7 +3603,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -3614,7 +3623,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -3634,7 +3643,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -3654,7 +3663,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -3674,7 +3683,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -3691,7 +3700,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -3708,7 +3717,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -3725,7 +3734,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -3742,7 +3751,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -3759,7 +3768,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -3779,7 +3788,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -3799,7 +3808,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -3819,7 +3828,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -3836,7 +3845,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -3856,7 +3865,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -3873,7 +3882,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3890,7 +3899,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -3907,7 +3916,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -3927,7 +3936,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -3944,7 +3953,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -3964,7 +3973,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -3984,7 +3993,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -4001,7 +4010,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -4021,7 +4030,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -4038,7 +4047,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -4058,7 +4067,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>96</v>
       </c>
@@ -4075,7 +4084,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>97</v>
       </c>
@@ -4095,7 +4104,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>98</v>
       </c>
@@ -4112,7 +4121,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>99</v>
       </c>
@@ -4132,7 +4141,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>100</v>
       </c>
@@ -4152,7 +4161,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>101</v>
       </c>
@@ -4172,7 +4181,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>102</v>
       </c>
@@ -4192,7 +4201,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>103</v>
       </c>
@@ -4212,7 +4221,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>104</v>
       </c>
@@ -4232,7 +4241,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>105</v>
       </c>
@@ -4252,7 +4261,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>106</v>
       </c>
@@ -4272,7 +4281,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>107</v>
       </c>
@@ -4292,7 +4301,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>108</v>
       </c>
@@ -4312,7 +4321,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>109</v>
       </c>
@@ -4332,7 +4341,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>110</v>
       </c>
@@ -4352,7 +4361,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>111</v>
       </c>
@@ -4369,7 +4378,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -4386,7 +4395,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -4406,7 +4415,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -4426,7 +4435,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -4446,7 +4455,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -4466,7 +4475,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -4486,7 +4495,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -4503,7 +4512,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -4523,7 +4532,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -4543,7 +4552,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -4563,7 +4572,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -4580,7 +4589,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -4600,7 +4609,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -4617,7 +4626,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -4637,7 +4646,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -4657,7 +4666,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
@@ -4674,7 +4683,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>128</v>
       </c>
@@ -4694,7 +4703,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>129</v>
       </c>
@@ -4714,7 +4723,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>130</v>
       </c>
@@ -4734,7 +4743,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>131</v>
       </c>
@@ -4751,7 +4760,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>132</v>
       </c>
@@ -4771,7 +4780,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>133</v>
       </c>
@@ -4788,7 +4797,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>134</v>
       </c>
@@ -4808,7 +4817,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>135</v>
       </c>
@@ -4828,7 +4837,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>136</v>
       </c>
@@ -4845,7 +4854,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>137</v>
       </c>
@@ -4865,7 +4874,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>138</v>
       </c>
@@ -4885,7 +4894,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>139</v>
       </c>
@@ -4902,7 +4911,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>140</v>
       </c>
@@ -4919,7 +4928,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>141</v>
       </c>
@@ -4936,7 +4945,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>142</v>
       </c>
@@ -4956,7 +4965,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>143</v>
       </c>
@@ -4976,7 +4985,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>144</v>
       </c>
@@ -4996,7 +5005,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>145</v>
       </c>
@@ -5016,7 +5025,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>146</v>
       </c>
@@ -5036,7 +5045,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>147</v>
       </c>
@@ -5053,7 +5062,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>148</v>
       </c>
@@ -5073,7 +5082,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>149</v>
       </c>
@@ -5093,7 +5102,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>150</v>
       </c>
@@ -5110,7 +5119,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>151</v>
       </c>
@@ -5127,7 +5136,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>152</v>
       </c>
@@ -5147,7 +5156,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>153</v>
       </c>
@@ -5167,7 +5176,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>154</v>
       </c>
@@ -5187,7 +5196,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>155</v>
       </c>
@@ -5207,7 +5216,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
@@ -5224,7 +5233,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>157</v>
       </c>
@@ -5244,7 +5253,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>158</v>
       </c>
@@ -5264,7 +5273,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>159</v>
       </c>
@@ -5284,7 +5293,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
@@ -5304,7 +5313,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
@@ -5324,7 +5333,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
@@ -5344,7 +5353,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
@@ -5364,7 +5373,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
@@ -5384,7 +5393,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
@@ -5404,7 +5413,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
@@ -5424,7 +5433,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
@@ -5444,7 +5453,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -5468,7 +5477,7 @@
         <v>Rsrv_Gain_empty</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
@@ -5488,7 +5497,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
@@ -5508,7 +5517,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
@@ -5528,7 +5537,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
@@ -5548,7 +5557,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
@@ -5568,7 +5577,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
@@ -5588,7 +5597,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
@@ -5608,7 +5617,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
@@ -5632,7 +5641,7 @@
         <v>Frm_Gain</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
@@ -5656,7 +5665,7 @@
         <v>Frm_Gain_empty</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
@@ -5676,7 +5685,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
@@ -5700,7 +5709,7 @@
         <v>NPGain_FrmGain</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
@@ -5720,7 +5729,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
@@ -5740,7 +5749,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
@@ -5760,7 +5769,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
@@ -5780,7 +5789,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
@@ -5800,7 +5809,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
@@ -5820,7 +5829,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
@@ -5840,7 +5849,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
@@ -5860,7 +5869,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
@@ -5883,7 +5892,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
@@ -5903,7 +5912,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
@@ -5923,7 +5932,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
@@ -5943,7 +5952,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
@@ -5967,7 +5976,7 @@
         <v>An_NDF</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
@@ -5991,7 +6000,7 @@
         <v>Fe_CPend_g</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
@@ -6015,7 +6024,7 @@
         <v>Fe_CPend</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
@@ -6035,7 +6044,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
@@ -6055,7 +6064,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
@@ -6075,7 +6084,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
@@ -6099,7 +6108,7 @@
         <v>Scrf_CP_g</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
@@ -6119,7 +6128,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
@@ -6139,7 +6148,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>201</v>
       </c>
@@ -6159,7 +6168,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>202</v>
       </c>
@@ -6179,7 +6188,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>203</v>
       </c>
@@ -6199,7 +6208,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>204</v>
       </c>
@@ -6219,7 +6228,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>205</v>
       </c>
@@ -6243,7 +6252,7 @@
         <v>CPGain_FrmGain</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>206</v>
       </c>
@@ -6267,7 +6276,7 @@
         <v>NPGain_FrmGain</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>207</v>
       </c>
@@ -6291,7 +6300,7 @@
         <v>Frm_Gain</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>208</v>
       </c>
@@ -6315,7 +6324,7 @@
         <v>Frm_Gain_empty</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>209</v>
       </c>
@@ -6339,7 +6348,7 @@
         <v>Frm_NPgain</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>210</v>
       </c>
@@ -6363,7 +6372,7 @@
         <v>NPGain_RsrvGain</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>211</v>
       </c>
@@ -6387,7 +6396,7 @@
         <v>Rsrv_Gain_empty</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>212</v>
       </c>
@@ -6411,7 +6420,7 @@
         <v>Rsrv_NPgain</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>213</v>
       </c>
@@ -6435,7 +6444,7 @@
         <v>Body_NPgain</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>214</v>
       </c>
@@ -6455,7 +6464,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>215</v>
       </c>
@@ -6475,7 +6484,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>216</v>
       </c>
@@ -6499,7 +6508,7 @@
         <v>Gest_NCPgain_g</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>217</v>
       </c>
@@ -6523,7 +6532,7 @@
         <v>Gest_NPgain_g</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>218</v>
       </c>
@@ -6547,7 +6556,7 @@
         <v>Gest_NPuse_g</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>219</v>
       </c>
@@ -6567,7 +6576,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>220</v>
       </c>
@@ -6587,7 +6596,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>221</v>
       </c>
@@ -6607,7 +6616,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>222</v>
       </c>
@@ -6624,7 +6633,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>223</v>
       </c>
@@ -6644,7 +6653,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>224</v>
       </c>
@@ -6664,7 +6673,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>225</v>
       </c>
@@ -6684,7 +6693,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>226</v>
       </c>
@@ -6704,7 +6713,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="228" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>227</v>
       </c>
@@ -6724,7 +6733,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="229" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>228</v>
       </c>
@@ -6744,7 +6753,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="230" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>229</v>
       </c>
@@ -6764,7 +6773,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="231" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>230</v>
       </c>
@@ -6784,7 +6793,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="232" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>231</v>
       </c>
@@ -6804,7 +6813,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="233" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B233" t="s">
         <v>523</v>
       </c>
@@ -6812,7 +6821,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B234" t="s">
         <v>525</v>
       </c>
@@ -6820,7 +6829,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>232</v>
       </c>
@@ -6837,7 +6846,7 @@
         <v>2689</v>
       </c>
     </row>
-    <row r="236" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>233</v>
       </c>
@@ -6854,7 +6863,7 @@
         <v>2686</v>
       </c>
     </row>
-    <row r="237" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>234</v>
       </c>
@@ -6868,7 +6877,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>235</v>
       </c>
@@ -6882,7 +6891,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="239" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>236</v>
       </c>
@@ -6896,7 +6905,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="240" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>237</v>
       </c>
@@ -6910,7 +6919,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>238</v>
       </c>
@@ -6924,7 +6933,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>239</v>
       </c>
@@ -6938,7 +6947,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>240</v>
       </c>
@@ -6964,20 +6973,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750FF422-2362-464E-8AF6-B12F418D3E4F}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="67.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="67.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>293</v>
       </c>
@@ -6988,7 +6997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>294</v>
       </c>
@@ -6999,7 +7008,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>296</v>
       </c>
@@ -7010,7 +7019,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>298</v>
       </c>
@@ -7021,7 +7030,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>299</v>
       </c>
@@ -7032,7 +7041,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>301</v>
       </c>
@@ -7043,7 +7052,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>302</v>
       </c>
@@ -7054,7 +7063,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>309</v>
       </c>
@@ -7065,7 +7074,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>311</v>
       </c>
@@ -7076,7 +7085,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>314</v>
       </c>
@@ -7087,7 +7096,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>318</v>
       </c>
@@ -7098,7 +7107,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>320</v>
       </c>
@@ -7109,7 +7118,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>322</v>
       </c>
@@ -7120,7 +7129,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>323</v>
       </c>
@@ -7131,7 +7140,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>325</v>
       </c>
@@ -7142,7 +7151,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>329</v>
       </c>
@@ -7153,7 +7162,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>331</v>
       </c>
@@ -7164,7 +7173,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>333</v>
       </c>
@@ -7175,7 +7184,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>335</v>
       </c>
@@ -7186,7 +7195,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>337</v>
       </c>
@@ -7197,7 +7206,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>339</v>
       </c>
@@ -7206,6 +7215,17 @@
       </c>
       <c r="C21" t="s">
         <v>340</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>535</v>
+      </c>
+      <c r="B22" t="s">
+        <v>536</v>
+      </c>
+      <c r="C22" t="s">
+        <v>537</v>
       </c>
     </row>
   </sheetData>

</xml_diff>